<commit_message>
(hopefully) function genetic gerrymandering algorithm finished
</commit_message>
<xml_diff>
--- a/human_readable_data.xlsx
+++ b/human_readable_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\menga\Downloads\Documents\Classes\CS\Gerrymandering\Gerrymandering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6959441-F9D2-4440-8191-8ABEF746779C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53ADB31-0379-4A2F-A199-329938AA9BBD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{50C5BEA9-7819-4B1A-A465-31B96CD9E9A9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="63">
   <si>
     <t>Women</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Trump Vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender Gap: </t>
   </si>
 </sst>
 </file>
@@ -564,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45FA5B6-5670-4A1D-B021-4B64996CE7B5}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2120,6 +2123,9 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>62</v>
+      </c>
       <c r="H54">
         <f>AVERAGE(H2:H51)</f>
         <v>8.6666666666666684E-2</v>

</xml_diff>